<commit_message>
Auswertung Bügelmethode fertig :D
</commit_message>
<xml_diff>
--- a/E4 Programmierung/Versuchsteil_C.xlsx
+++ b/E4 Programmierung/Versuchsteil_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ccb2a2ecf688a24/Dokumente/1 UNI/3. Sem/GP Physik/Grundpraktikum/E4 Programmierung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6A55AD50-2058-4E7F-8367-863440ADD574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{122F76F4-952F-4E98-AA8E-7248A014997A}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6A55AD50-2058-4E7F-8367-863440ADD574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89BC1084-F713-4B1A-9CBB-84C0231B7682}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{59891A01-AE5D-4455-915C-4A8C655A9C2A}"/>
+    <workbookView minimized="1" xWindow="5130" yWindow="3967" windowWidth="15390" windowHeight="9713" xr2:uid="{59891A01-AE5D-4455-915C-4A8C655A9C2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Versuchsteil_C" sheetId="1" r:id="rId1"/>
@@ -642,6 +642,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -944,12 +948,12 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +982,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1031,7 +1035,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>209.2</v>
       </c>
@@ -1088,7 +1092,7 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>317.57</v>
       </c>
@@ -1148,7 +1152,7 @@
         <v>0.40536679401158621</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>388.17</v>
       </c>
@@ -1208,7 +1212,7 @@
         <v>0.25132741228718347</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>431.22</v>
       </c>
@@ -1268,7 +1272,7 @@
         <v>3.5513656084058529</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>513.04999999999995</v>
       </c>
@@ -1328,7 +1332,7 @@
         <v>3.6376335988934447</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>565.42999999999995</v>
       </c>
@@ -1388,7 +1392,7 @@
         <v>3.4906585039886591</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>668.53</v>
       </c>
@@ -1448,7 +1452,7 @@
         <v>0.20943951023931953</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>623.49</v>
       </c>
@@ -1508,7 +1512,7 @@
         <v>0.39269908169872414</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>623.49</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>0.20943951023931953</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>724.26</v>
       </c>
@@ -1628,7 +1632,7 @@
         <v>0.23271056693257725</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>809.02</v>
       </c>
@@ -1688,7 +1692,7 @@
         <v>3.4033920413889422</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>878.64</v>
       </c>
@@ -1748,7 +1752,7 @@
         <v>0.54636393975474662</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>950.81</v>
       </c>
@@ -1808,7 +1812,7 @@
         <v>3.5903916041026207</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1070.5</v>
       </c>
@@ -1868,7 +1872,7 @@
         <v>0.69813170079773179</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1130.5</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>4.4351896285973549</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1242.0999999999999</v>
       </c>
@@ -1988,7 +1992,7 @@
         <v>5.497787143782138</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1311.1</v>
       </c>
@@ -2048,7 +2052,7 @@
         <v>5.8643062867009474</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1412.1</v>
       </c>
@@ -2108,7 +2112,7 @@
         <v>5.8343863566667586</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1519.8</v>
       </c>
@@ -2168,7 +2172,7 @@
         <v>5.7998633604734646</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>776.09</v>
       </c>
@@ -2228,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>600.37</v>
       </c>
@@ -2288,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>400.6</v>
       </c>
@@ -2348,7 +2352,7 @@
         <v>6.0318578948924024</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>263.2</v>
       </c>
@@ -2408,7 +2412,7 @@
         <v>5.6217973801080507</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>999.31</v>
       </c>
@@ -2468,7 +2472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>684.42</v>
       </c>

</xml_diff>